<commit_message>
fixed issue with FPRA in figures, removed renormalization after filtering and divided by actual sum of RA_obs. Need to implement in pipeline plotting an assigned higher pct.
</commit_message>
<xml_diff>
--- a/pipelines/nist/expected.xlsx
+++ b/pipelines/nist/expected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valenciaem/coding/pipelines/pipelines/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993773C6-3A6D-E04C-BF86-74AD7FA92897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0408A9BE-D7CB-7045-8614-FCB793368291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{6D54DD13-776B-5A4A-9E05-C8ACB8E35F39}"/>
   </bookViews>
@@ -79,15 +79,6 @@
     <t>Mix-A</t>
   </si>
   <si>
-    <t>MixB</t>
-  </si>
-  <si>
-    <t>MixC</t>
-  </si>
-  <si>
-    <t>MixD</t>
-  </si>
-  <si>
     <t>Pool A</t>
   </si>
   <si>
@@ -198,6 +189,15 @@
   </si>
   <si>
     <t>Salmonella enterica subsp. enterica</t>
+  </si>
+  <si>
+    <t>Mix-B</t>
+  </si>
+  <si>
+    <t>Mix-C</t>
+  </si>
+  <si>
+    <t>Mix-D</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,24 +599,24 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>884</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>884</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>884</v>
@@ -691,13 +691,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>768</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>768</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>768</v>
@@ -772,13 +772,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>728</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>728</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>728</v>
@@ -853,13 +853,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>970</v>
@@ -882,10 +882,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>970</v>
@@ -908,10 +908,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>970</v>
@@ -934,13 +934,13 @@
     </row>
     <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>1363</v>
@@ -963,10 +963,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>1363</v>

</xml_diff>